<commit_message>
Edited Visualization and excel generation
</commit_message>
<xml_diff>
--- a/target/classes/excel_files/StudentProgress_1.xlsx
+++ b/target/classes/excel_files/StudentProgress_1.xlsx
@@ -92,7 +92,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -123,27 +123,13 @@
         <v>3.0</v>
       </c>
       <c r="B2" t="n" s="0">
-        <v>100.0</v>
+        <v>0.0</v>
       </c>
-      <c r="C2" t="e" s="0">
-        <v>#NUM!</v>
+      <c r="C2" t="n" s="0">
+        <v>61.50000000000001</v>
       </c>
       <c r="D2" t="n" s="0">
-        <v>100.0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n" s="0">
-        <v>4.0</v>
-      </c>
-      <c r="B3" t="n" s="0">
-        <v>100.0</v>
-      </c>
-      <c r="C3" t="e" s="0">
-        <v>#NUM!</v>
-      </c>
-      <c r="D3" t="n" s="0">
-        <v>100.0</v>
+        <v>0.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>